<commit_message>
Parallel Test Report Generation
</commit_message>
<xml_diff>
--- a/ComcastCRMGUIFramework/testdata/TestscriptData.xlsx
+++ b/ComcastCRMGUIFramework/testdata/TestscriptData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="242">
   <si>
     <t>TC_ID</t>
   </si>
@@ -741,6 +741,21 @@
   </si>
   <si>
     <t>ACC40144</t>
+  </si>
+  <si>
+    <t>CON23858</t>
+  </si>
+  <si>
+    <t>CON23859</t>
+  </si>
+  <si>
+    <t>ACC40209</t>
+  </si>
+  <si>
+    <t>ACC40211</t>
+  </si>
+  <si>
+    <t>CON23862</t>
   </si>
 </sst>
 </file>
@@ -1588,7 +1603,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1656,7 +1671,7 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -1707,7 +1722,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1741,7 +1756,7 @@
         <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1775,7 +1790,7 @@
         <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>